<commit_message>
Thomas v005 with rough transitions
</commit_message>
<xml_diff>
--- a/Thomas.xlsx
+++ b/Thomas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19110" windowHeight="12840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19110" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="masuanaga-002.mvn" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,6 +515,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -545,7 +569,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -568,18 +592,23 @@
     <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,10 +955,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A41" activePane="bottomLeft"/>
-      <selection activeCell="B2" sqref="B2:D2"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <pane ySplit="600" activePane="bottomLeft"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -983,7 +1012,7 @@
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="26" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1016,7 +1045,7 @@
         <f t="shared" si="1"/>
         <v>1311</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="27" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1034,6 +1063,7 @@
         <f t="shared" si="1"/>
         <v>2228</v>
       </c>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
@@ -1046,12 +1076,14 @@
         <f t="shared" si="1"/>
         <v>2274.75</v>
       </c>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:5">
       <c r="C11" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="8" t="s">
@@ -1064,7 +1096,7 @@
         <f t="shared" si="1"/>
         <v>2279.25</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="27" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1082,12 +1114,14 @@
         <f t="shared" si="1"/>
         <v>2870.25</v>
       </c>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:5">
       <c r="C14" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
@@ -1100,7 +1134,7 @@
         <f t="shared" si="1"/>
         <v>2878</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="27" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1118,6 +1152,7 @@
         <f t="shared" si="1"/>
         <v>3477.75</v>
       </c>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="1:5">
       <c r="C17" s="3">
@@ -1309,7 +1344,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="26" t="s">
         <v>51</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -1363,7 +1398,7 @@
         <f t="shared" ref="C41" si="4">B41/4</f>
         <v>91.25</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="26" t="s">
         <v>64</v>
       </c>
       <c r="F41" s="19"/>
@@ -1399,7 +1434,7 @@
         <f t="shared" si="5"/>
         <v>5513.25</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="26" t="s">
         <v>65</v>
       </c>
       <c r="F44" s="19"/>
@@ -1434,7 +1469,7 @@
         <f t="shared" si="5"/>
         <v>8476.75</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="28" t="s">
         <v>66</v>
       </c>
       <c r="G47" s="19"/>
@@ -1470,7 +1505,7 @@
         <f t="shared" si="5"/>
         <v>9942</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="28" t="s">
         <v>67</v>
       </c>
       <c r="G50" s="19"/>
@@ -1506,7 +1541,7 @@
         <f t="shared" si="5"/>
         <v>11152</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="28" t="s">
         <v>68</v>
       </c>
       <c r="G53" s="19"/>
@@ -1542,7 +1577,7 @@
         <f t="shared" si="5"/>
         <v>12270.75</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" s="28" t="s">
         <v>55</v>
       </c>
       <c r="G56" s="19"/>
@@ -1577,7 +1612,7 @@
         <f t="shared" si="5"/>
         <v>13743</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" s="28" t="s">
         <v>69</v>
       </c>
       <c r="H59" s="19"/>
@@ -1613,7 +1648,7 @@
         <f t="shared" si="7"/>
         <v>15483.25</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H62" s="19"/>
@@ -1636,7 +1671,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I64" s="24"/>
+      <c r="I64" s="22"/>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
@@ -1652,7 +1687,7 @@
       <c r="E65" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I65" s="24"/>
+      <c r="I65" s="22"/>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
@@ -1665,7 +1700,7 @@
         <f t="shared" si="7"/>
         <v>19527.5</v>
       </c>
-      <c r="I66" s="24"/>
+      <c r="I66" s="22"/>
     </row>
     <row r="67" spans="1:9">
       <c r="C67" s="3">
@@ -1716,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="BA3" sqref="BA3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1760,12 +1795,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:57">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="15"/>
       <c r="I2" s="13" t="s">
         <v>84</v>
@@ -1775,45 +1810,45 @@
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="W2" s="20" t="s">
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="W2" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AH2" s="20" t="s">
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30"/>
+      <c r="AH2" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AM2" s="20" t="s">
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="30"/>
+      <c r="AM2" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
+      <c r="AN2" s="30"/>
+      <c r="AO2" s="30"/>
       <c r="AR2" t="s">
         <v>115</v>
       </c>
-      <c r="AZ2" s="26" t="s">
+      <c r="AZ2" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="BA2" s="26"/>
-      <c r="BB2" s="26"/>
-      <c r="BC2" s="26"/>
-      <c r="BD2" s="26"/>
+      <c r="BA2" s="29"/>
+      <c r="BB2" s="29"/>
+      <c r="BC2" s="29"/>
+      <c r="BD2" s="29"/>
     </row>
     <row r="3" spans="1:57">
       <c r="B3" t="s">
@@ -1825,7 +1860,7 @@
       <c r="D3" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="25" t="s">
         <v>53</v>
       </c>
       <c r="F3" t="s">
@@ -1861,7 +1896,7 @@
       <c r="Q3" t="s">
         <v>123</v>
       </c>
-      <c r="R3" s="25" t="str">
+      <c r="R3" s="23" t="str">
         <f>"Clip" &amp; M3</f>
         <v>ClipLongMasunaga</v>
       </c>
@@ -1989,7 +2024,7 @@
       <c r="D4" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="25" t="s">
         <v>54</v>
       </c>
       <c r="F4" t="s">
@@ -2025,7 +2060,7 @@
       <c r="Q4" t="s">
         <v>123</v>
       </c>
-      <c r="R4" s="25" t="str">
+      <c r="R4" s="23" t="str">
         <f t="shared" ref="R4:R24" si="3">"Clip" &amp; M4</f>
         <v>ClipMaagStarking</v>
       </c>
@@ -2153,7 +2188,7 @@
       <c r="D5" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="25" t="s">
         <v>83</v>
       </c>
       <c r="F5" t="s">
@@ -2189,7 +2224,7 @@
       <c r="Q5" t="s">
         <v>123</v>
       </c>
-      <c r="R5" s="25" t="str">
+      <c r="R5" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipHart1</v>
       </c>
@@ -2317,7 +2352,7 @@
       <c r="D6" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="25" t="s">
         <v>56</v>
       </c>
       <c r="F6" t="s">
@@ -2353,7 +2388,7 @@
       <c r="Q6" t="s">
         <v>123</v>
       </c>
-      <c r="R6" s="25" t="str">
+      <c r="R6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipBlaas</v>
       </c>
@@ -2481,7 +2516,7 @@
       <c r="D7" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="24" t="s">
         <v>57</v>
       </c>
       <c r="F7" t="s">
@@ -2517,7 +2552,7 @@
       <c r="Q7" t="s">
         <v>123</v>
       </c>
-      <c r="R7" s="25" t="str">
+      <c r="R7" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipZwing</v>
       </c>
@@ -2645,7 +2680,7 @@
       <c r="D8" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="24" t="s">
         <v>58</v>
       </c>
       <c r="F8" t="s">
@@ -2681,7 +2716,7 @@
       <c r="Q8" t="s">
         <v>123</v>
       </c>
-      <c r="R8" s="25" t="str">
+      <c r="R8" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipLever</v>
       </c>
@@ -2809,7 +2844,7 @@
       <c r="D9" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="24" t="s">
         <v>59</v>
       </c>
       <c r="F9" t="s">
@@ -2845,7 +2880,7 @@
       <c r="Q9" t="s">
         <v>123</v>
       </c>
-      <c r="R9" s="25" t="str">
+      <c r="R9" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipKantStreking</v>
       </c>
@@ -2973,7 +3008,7 @@
       <c r="D10" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="24" t="s">
         <v>81</v>
       </c>
       <c r="F10" t="s">
@@ -3009,7 +3044,7 @@
       <c r="Q10" t="s">
         <v>123</v>
       </c>
-      <c r="R10" s="25" t="str">
+      <c r="R10" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipBehandeling1</v>
       </c>
@@ -3173,7 +3208,7 @@
       <c r="Q11" t="s">
         <v>123</v>
       </c>
-      <c r="R11" s="25" t="str">
+      <c r="R11" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipMasunaga2</v>
       </c>
@@ -3337,7 +3372,7 @@
       <c r="Q12" t="s">
         <v>123</v>
       </c>
-      <c r="R12" s="25" t="str">
+      <c r="R12" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipMasunaga3</v>
       </c>
@@ -3465,7 +3500,7 @@
       <c r="D13" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="20" t="s">
         <v>62</v>
       </c>
       <c r="F13" t="s">
@@ -3501,7 +3536,7 @@
       <c r="Q13" t="s">
         <v>123</v>
       </c>
-      <c r="R13" s="25" t="str">
+      <c r="R13" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipMasunaga4</v>
       </c>
@@ -3665,7 +3700,7 @@
       <c r="Q14" t="s">
         <v>123</v>
       </c>
-      <c r="R14" s="25" t="str">
+      <c r="R14" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipWarmingUp</v>
       </c>
@@ -3793,7 +3828,7 @@
       <c r="D15" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="21" t="s">
         <v>65</v>
       </c>
       <c r="F15" t="s">
@@ -3829,7 +3864,7 @@
       <c r="Q15" t="s">
         <v>123</v>
       </c>
-      <c r="R15" s="25" t="str">
+      <c r="R15" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipLong</v>
       </c>
@@ -3993,7 +4028,7 @@
       <c r="Q16" t="s">
         <v>123</v>
       </c>
-      <c r="R16" s="25" t="str">
+      <c r="R16" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipMaag</v>
       </c>
@@ -4121,7 +4156,7 @@
       <c r="D17" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="22" t="s">
         <v>67</v>
       </c>
       <c r="F17" t="s">
@@ -4157,7 +4192,7 @@
       <c r="Q17" t="s">
         <v>123</v>
       </c>
-      <c r="R17" s="25" t="str">
+      <c r="R17" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipNier</v>
       </c>
@@ -4321,7 +4356,7 @@
       <c r="Q18" t="s">
         <v>123</v>
       </c>
-      <c r="R18" s="25" t="str">
+      <c r="R18" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipWarmer</v>
       </c>
@@ -4485,7 +4520,7 @@
       <c r="Q19" t="s">
         <v>123</v>
       </c>
-      <c r="R19" s="25" t="str">
+      <c r="R19" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipHart2</v>
       </c>
@@ -4649,7 +4684,7 @@
       <c r="Q20" t="s">
         <v>123</v>
       </c>
-      <c r="R20" s="25" t="str">
+      <c r="R20" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipRugSterking</v>
       </c>
@@ -4813,7 +4848,7 @@
       <c r="Q21" t="s">
         <v>123</v>
       </c>
-      <c r="R21" s="25" t="str">
+      <c r="R21" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipLeverSterking</v>
       </c>
@@ -4941,7 +4976,7 @@
       <c r="D22" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="22" t="s">
         <v>71</v>
       </c>
       <c r="F22" t="s">
@@ -4977,7 +5012,7 @@
       <c r="Q22" t="s">
         <v>123</v>
       </c>
-      <c r="R22" s="25" t="str">
+      <c r="R22" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipBehandeling2</v>
       </c>
@@ -5141,7 +5176,7 @@
       <c r="Q23" t="s">
         <v>123</v>
       </c>
-      <c r="R23" s="25" t="str">
+      <c r="R23" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipBehandeling3</v>
       </c>
@@ -5305,7 +5340,7 @@
       <c r="Q24" t="s">
         <v>123</v>
       </c>
-      <c r="R24" s="25" t="str">
+      <c r="R24" s="23" t="str">
         <f t="shared" si="3"/>
         <v>ClipStop</v>
       </c>

</xml_diff>